<commit_message>
added allocrule 1 net loss tests
</commit_message>
<xml_diff>
--- a/ftest/data/fm24/allocrule1_results.xlsx
+++ b/ftest/data/fm24/allocrule1_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64_2\home\Joh\ktest\ftest\data\fm24\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64\home\Joh\ktest\ftest\data\fm24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35428C9C-E0F9-45B8-A984-2293F8E3E6FF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDCBE6BD-20F5-457F-9AD8-36218ADE1B3C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{6A789974-1291-4E83-A431-41144F7FC8D7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6A789974-1291-4E83-A431-41144F7FC8D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,14 +88,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -400,15 +410,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB383C4-5CED-4CCF-800B-EEB5AA2962FC}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -416,7 +430,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -436,7 +450,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>1</v>
       </c>
@@ -449,8 +463,15 @@
       <c r="E4">
         <v>7211247</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F4">
+        <v>3751520.25</v>
+      </c>
+      <c r="G4">
+        <v>2108149.75</v>
+      </c>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>2</v>
       </c>
@@ -463,8 +484,15 @@
       <c r="E5">
         <v>7211247</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F5">
+        <v>3751520.25</v>
+      </c>
+      <c r="G5">
+        <v>2108149.75</v>
+      </c>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>3</v>
       </c>
@@ -477,8 +505,15 @@
       <c r="E6">
         <v>4322077.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F6">
+        <v>2248482.25</v>
+      </c>
+      <c r="G6">
+        <v>1263524.3799999999</v>
+      </c>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>4</v>
       </c>
@@ -491,8 +526,15 @@
       <c r="E7">
         <v>1255429.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F7">
+        <v>653114.38</v>
+      </c>
+      <c r="G7">
+        <v>367014.66</v>
+      </c>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>5</v>
       </c>
@@ -505,8 +547,15 @@
       <c r="E8">
         <v>75283624</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F8">
+        <v>39164936</v>
+      </c>
+      <c r="G8">
+        <v>22008558</v>
+      </c>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>6</v>
       </c>
@@ -519,8 +568,15 @@
       <c r="E9">
         <v>28382156</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F9">
+        <v>14765301</v>
+      </c>
+      <c r="G9">
+        <v>8297294</v>
+      </c>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>7</v>
       </c>
@@ -533,8 +589,15 @@
       <c r="E10">
         <v>575000</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F10">
+        <v>299133.31</v>
+      </c>
+      <c r="G10">
+        <v>168096.59</v>
+      </c>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>8</v>
       </c>
@@ -547,8 +610,15 @@
       <c r="E11">
         <v>15000000</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F11">
+        <v>7803477.5</v>
+      </c>
+      <c r="G11">
+        <v>4385129</v>
+      </c>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>9</v>
       </c>
@@ -561,8 +631,15 @@
       <c r="E12">
         <v>79200000</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F12">
+        <v>41202360</v>
+      </c>
+      <c r="G12">
+        <v>23153478</v>
+      </c>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>10</v>
       </c>
@@ -575,6 +652,13 @@
       <c r="E13">
         <v>31680000</v>
       </c>
+      <c r="F13">
+        <v>16480944</v>
+      </c>
+      <c r="G13">
+        <v>9261392</v>
+      </c>
+      <c r="K13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>